<commit_message>
Updated Tidy Table, Master Template, and Submissions folder
</commit_message>
<xml_diff>
--- a/in-progress/L112_Tuncer_2006_Nanotechnology/L112_Tuncer_TT.xlsx
+++ b/in-progress/L112_Tuncer_2006_Nanotechnology/L112_Tuncer_TT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/wishlist/L112_Tuncer_2006_Nanotechnology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/in-progress/L112_Tuncer_2006_Nanotechnology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84116CFC-100D-084A-BCDE-C7A8E80D8837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637DC1A-8B48-7645-A7BB-D1BB8C8B3EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D8BD3E46-8F3E-9D47-84CF-EE9ACAD4FE4C}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,62 +613,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>5</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>6</v>
+      <c r="C3" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>7</v>
+      <c r="C4" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>8</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>

</xml_diff>